<commit_message>
add contact manage module and send email feature
</commit_message>
<xml_diff>
--- a/Document/Excel Status Report/eProject_Status_Report _TonThatThanhLong.xlsx
+++ b/Document/Excel Status Report/eProject_Status_Report _TonThatThanhLong.xlsx
@@ -1,48 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView windowWidth="20490" windowHeight="7965"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Trang tính1" sheetId="1" r:id="rId4"/>
+    <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <r>
       <rPr>
-        <rFont val="Verdana"/>
         <b/>
         <i/>
+        <u/>
+        <sz val="12"/>
         <color rgb="FFFF0000"/>
-        <sz val="12.0"/>
-        <u/>
+        <rFont val="Verdana"/>
+        <charset val="134"/>
       </rPr>
       <t>Note :</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Verdana"/>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-        <sz val="12.0"/>
-        <u/>
+        <charset val="134"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
         <rFont val="Verdana"/>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0000FF"/>
-        <sz val="12.0"/>
-        <u/>
+        <charset val="134"/>
       </rPr>
       <t>Kindly go through the Read Me.txt file, which is available in the project specification Zip folder.</t>
     </r>
@@ -73,6 +77,9 @@
   </si>
   <si>
     <t>Curriculum</t>
+  </si>
+  <si>
+    <t>OV-6715-ACCP-ADSE</t>
   </si>
   <si>
     <t>Semester</t>
@@ -162,66 +169,255 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="dd\-mmm\-yyyy"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10">
-    <font>
-      <sz val="10.0"/>
+  <fonts count="32">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <i/>
       <u/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Verdana"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="SimSun"/>
-    </font>
-    <font/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Verdana"/>
-    </font>
-    <font>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Verdana"/>
-    </font>
-    <font>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Verdana"/>
+      <charset val="134"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -229,9 +425,201 @@
         <bgColor rgb="FFFFFF99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
-    <border/>
+  <borders count="21">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -245,58 +633,87 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -308,6 +725,8 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -316,6 +735,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -324,105 +746,378 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellXfs count="30">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="8" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="178" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -612,52 +1307,56 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
-    <col customWidth="1" min="2" max="2" width="42.43"/>
-    <col customWidth="1" min="3" max="3" width="50.43"/>
-    <col customWidth="1" min="4" max="4" width="63.29"/>
-    <col customWidth="1" min="5" max="6" width="14.43"/>
+    <col min="1" max="1" width="14.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="42.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="50.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="63.2857142857143" customWidth="1"/>
+    <col min="5" max="6" width="14.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" ht="15.75" customHeight="1" spans="1:5">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" ht="15.75" customHeight="1" spans="1:5">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" ht="15.75" customHeight="1" spans="1:5">
       <c r="A3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" ht="15.75" customHeight="1" spans="1:5">
       <c r="A4" s="1"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" ht="15.75" customHeight="1" spans="1:5">
       <c r="A5" s="4"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -666,20 +1365,20 @@
       <c r="D5" s="8"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" ht="15.75" customHeight="1" spans="1:5">
       <c r="A6" s="4"/>
       <c r="B6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" ht="15.75" customHeight="1" spans="1:5">
       <c r="A7" s="4"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" ht="15.75" customHeight="1" spans="1:5">
       <c r="A8" s="5"/>
       <c r="B8" s="14" t="s">
         <v>2</v>
@@ -692,7 +1391,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" ht="15.75" customHeight="1" spans="1:5">
       <c r="A9" s="5"/>
       <c r="B9" s="17"/>
       <c r="C9" s="18" t="s">
@@ -703,7 +1402,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" ht="15.75" customHeight="1" spans="1:5">
       <c r="A10" s="5"/>
       <c r="B10" s="17"/>
       <c r="C10" s="18" t="s">
@@ -714,246 +1413,248 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" ht="15.75" customHeight="1" spans="1:5">
       <c r="A11" s="5"/>
       <c r="B11" s="17"/>
       <c r="C11" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="16"/>
+      <c r="D11" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" ht="15.75" customHeight="1" spans="1:5">
       <c r="A12" s="5"/>
       <c r="B12" s="17"/>
       <c r="C12" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="21" t="s">
         <v>11</v>
       </c>
+      <c r="D12" s="16" t="s">
+        <v>12</v>
+      </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" ht="15.75" customHeight="1" spans="1:5">
       <c r="A13" s="5"/>
-      <c r="B13" s="22"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" ht="15.75" customHeight="1" spans="1:5">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" ht="15.75" customHeight="1" spans="1:5">
       <c r="A15" s="5"/>
       <c r="B15" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="23" t="s">
         <v>16</v>
       </c>
+      <c r="D15" s="22" t="s">
+        <v>17</v>
+      </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" ht="15.75" customHeight="1" spans="1:5">
       <c r="A16" s="5"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" ht="15.75" customHeight="1" spans="1:5">
       <c r="A17" s="5"/>
       <c r="B17" s="17"/>
-      <c r="C17" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="25">
-        <v>44320.0</v>
+      <c r="C17" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="24">
+        <v>44320</v>
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" ht="15.75" customHeight="1" spans="1:5">
       <c r="A18" s="5"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="26">
-        <v>44350.0</v>
+      <c r="B18" s="21"/>
+      <c r="C18" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="24">
+        <v>44350</v>
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" ht="15.75" customHeight="1" spans="1:5">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" ht="15.75" customHeight="1" spans="1:5">
       <c r="A20" s="4"/>
-      <c r="B20" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="28" t="s">
+      <c r="B20" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="C20" s="26" t="s">
         <v>22</v>
       </c>
+      <c r="D20" s="27" t="s">
+        <v>23</v>
+      </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" ht="15.75" customHeight="1" spans="1:5">
       <c r="A21" s="4"/>
       <c r="B21" s="17"/>
-      <c r="C21" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="25">
-        <v>44326.0</v>
+      <c r="C21" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="24">
+        <v>44326</v>
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" ht="15.75" customHeight="1" spans="1:5">
       <c r="A22" s="4"/>
       <c r="B22" s="17"/>
-      <c r="C22" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="31" t="s">
+      <c r="C22" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="32" t="s">
+      <c r="D22" s="27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
+      <c r="E22" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" customHeight="1" spans="1:5">
       <c r="A23" s="4"/>
       <c r="B23" s="17"/>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
+    </row>
+    <row r="24" ht="15.75" customHeight="1" spans="1:5">
       <c r="A24" s="4"/>
       <c r="B24" s="17"/>
-      <c r="C24" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="31" t="s">
+      <c r="C24" s="28" t="s">
         <v>29</v>
       </c>
+      <c r="D24" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" ht="15.75" customHeight="1" spans="1:5">
       <c r="A25" s="4"/>
       <c r="B25" s="17"/>
-      <c r="C25" s="30"/>
+      <c r="C25" s="28"/>
       <c r="D25" s="5"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" ht="15.75" customHeight="1" spans="1:5">
       <c r="A26" s="4"/>
       <c r="B26" s="17"/>
-      <c r="C26" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="31" t="s">
+      <c r="C26" s="26" t="s">
         <v>31</v>
       </c>
+      <c r="D26" s="27" t="s">
+        <v>32</v>
+      </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" ht="15.75" customHeight="1" spans="1:5">
       <c r="A27" s="4"/>
       <c r="B27" s="17"/>
-      <c r="C27" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="26">
-        <v>44344.0</v>
+      <c r="C27" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="24">
+        <v>44344</v>
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" ht="15.75" customHeight="1" spans="1:5">
       <c r="A28" s="4"/>
       <c r="B28" s="17"/>
-      <c r="C28" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="31" t="s">
-        <v>32</v>
+      <c r="C28" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>33</v>
       </c>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" ht="15.75" customHeight="1" spans="1:5">
       <c r="A29" s="4"/>
       <c r="B29" s="17"/>
-      <c r="C29" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>25</v>
+      <c r="C29" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>26</v>
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" ht="15.75" customHeight="1" spans="1:5">
       <c r="A30" s="4"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="31" t="s">
+      <c r="B30" s="21"/>
+      <c r="C30" s="28" t="s">
         <v>29</v>
       </c>
+      <c r="D30" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" ht="15.75" customHeight="1" spans="1:5">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="5"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" ht="15.75" customHeight="1" spans="1:5">
       <c r="A32" s="5"/>
       <c r="B32" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="31" t="s">
+      <c r="C32" s="29" t="s">
         <v>35</v>
       </c>
+      <c r="D32" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" ht="15.75" customHeight="1" spans="1:5">
       <c r="A33" s="4"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D33" s="31" t="s">
+      <c r="B33" s="21"/>
+      <c r="C33" s="29" t="s">
         <v>37</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>38</v>
       </c>
       <c r="E33" s="1"/>
     </row>
@@ -1926,16 +2627,17 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B2:D3"/>
-    <mergeCell ref="B5:D7"/>
     <mergeCell ref="B8:B13"/>
     <mergeCell ref="B15:B18"/>
     <mergeCell ref="B20:B30"/>
     <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="B5:D7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D10"/>
+    <hyperlink ref="D10" r:id="rId1" display="thanhlong005xtdl@gmail.com"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>